<commit_message>
Add HLOOKUP and improved tests for VLOOKUP.
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\workspace\koala\tests\ast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemonson/workspaces/koala/tests/ast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF73054-B405-45B0-8713-A9DF43A948E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8720B5FE-C5EA-794B-B242-7589C5D3E2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31400" yWindow="0" windowWidth="31360" windowHeight="21540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,14 @@
     <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
     <definedName name="NOP">Sheet1!$N$7:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Romain</t>
   </si>
@@ -70,9 +72,6 @@
     <t>lead guitar</t>
   </si>
   <si>
-    <t>rythm guitar</t>
-  </si>
-  <si>
     <t>drums</t>
   </si>
   <si>
@@ -80,6 +79,18 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Pay</t>
+  </si>
+  <si>
+    <t>rhythm guitar</t>
   </si>
 </sst>
 </file>
@@ -501,12 +512,12 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -557,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -601,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -641,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -652,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -669,12 +680,12 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -700,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>8</v>
       </c>
@@ -723,15 +734,15 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P11" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ref="A13:G13" si="2">EmptyRange</f>
         <v>0</v>
@@ -761,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -794,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>30</v>
       </c>
@@ -831,7 +842,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>20</v>
+      </c>
+      <c r="L20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -854,10 +887,10 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L22">
         <f>$H$22*20+I22</f>
@@ -876,7 +909,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
@@ -899,14 +932,26 @@
         <v>3</v>
       </c>
       <c r="K23" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L25" si="4">$H$22*20+I23</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <f>VLOOKUP("Pa??",J22:L25,3, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="O23">
+        <f>VLOOKUP("Ringo",J22:L25,3,FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="P23" t="e">
+        <f>VLOOKUP("Pual",J22:L25,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
@@ -926,17 +971,29 @@
         <v>30</v>
       </c>
       <c r="J24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <f>VLOOKUP("Pa",J22:L25,3)</f>
+        <v>40</v>
+      </c>
+      <c r="O24">
+        <f>VLOOKUP("Ringo",J22:L25,3)</f>
+        <v>60</v>
+      </c>
+      <c r="P24">
+        <f>VLOOKUP("Pual",J22:L25,3)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I25">
         <v>40</v>
       </c>
@@ -944,14 +1001,14 @@
         <v>5</v>
       </c>
       <c r="K25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L25">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B26" t="e">
         <f>A22:B24+A22:C22</f>
         <v>#VALUE!</v>
@@ -964,8 +1021,48 @@
         <f ca="1">SUM(OFFSET(A22,0,1):D22)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N26" t="str">
+        <f>HLOOKUP(22,J20:L25,4)</f>
+        <v>rhythm guitar</v>
+      </c>
+      <c r="O26">
+        <f>HLOOKUP(30,J20:L25,4,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="P26" t="e">
+        <f>HLOOKUP(31,J20:L25,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <f>HLOOKUP("Pa?",J21:L25,3, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="O27" t="str">
+        <f>HLOOKUP("Artist",J21:L25,3,FALSE)</f>
+        <v>John☺</v>
+      </c>
+      <c r="P27" t="e">
+        <f>HLOOKUP("Pya",J21:L25,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N28" t="str">
+        <f>HLOOKUP("Pa",J21:L25,3)</f>
+        <v>rhythm guitar</v>
+      </c>
+      <c r="O28" t="str">
+        <f>HLOOKUP("Instrument",J21:L25,3)</f>
+        <v>rhythm guitar</v>
+      </c>
+      <c r="P28">
+        <f>HLOOKUP("Pya",J21:L25,3)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C30">
         <v>1</v>
       </c>
@@ -979,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1003,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C32">
         <f>Liste5 +10</f>
         <v>12</v>
@@ -1021,7 +1118,7 @@
         <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L32" t="e">
         <f>MATCH(K31,K32:K33,1)</f>
@@ -1032,12 +1129,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1045,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f>2%+A36</f>
         <v>1.02</v>
@@ -1055,19 +1152,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="array" ref="A39">IFERROR(MATCH(TRUE,Liste&gt;2,0),"Rien")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>CHOOSE(A1, J22,J23,J24,J25)</f>
-        <v>Paul</v>
+        <v>George</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J22:K25">
+    <sortCondition ref="J22"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1082,17 +1182,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1101,47 +1201,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1150,47 +1250,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1213,9 +1313,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>

</xml_diff>